<commit_message>
Added 9V Calibration values and 3d printer manual.
</commit_message>
<xml_diff>
--- a/Documents/160628_Strain_Gages_Sensitivity.xlsx
+++ b/Documents/160628_Strain_Gages_Sensitivity.xlsx
@@ -9,13 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SG_Sensitivity" sheetId="5" r:id="rId1"/>
     <sheet name="470_Ohm_Meas" sheetId="1" r:id="rId2"/>
     <sheet name="750_Ohm_Meas" sheetId="4" r:id="rId3"/>
+    <sheet name="9V_Battery_Calibration" sheetId="7" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="40">
   <si>
     <t>Force [N]</t>
   </si>
@@ -126,6 +130,27 @@
   <si>
     <t>Arduino</t>
   </si>
+  <si>
+    <t>Weigth [Kg]</t>
+  </si>
+  <si>
+    <t>Weigth/2 [Kg]</t>
+  </si>
+  <si>
+    <t>Force/2 [N]</t>
+  </si>
+  <si>
+    <t>Arduino Int []</t>
+  </si>
+  <si>
+    <t>Arduino Volt. [N]</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
 </sst>
 </file>
 
@@ -172,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -180,12 +205,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -198,12 +285,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -231,6 +357,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -310,6 +437,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -398,11 +526,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-680721248"/>
-        <c:axId val="-680719616"/>
+        <c:axId val="811215728"/>
+        <c:axId val="811201584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-680721248"/>
+        <c:axId val="811215728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -459,12 +587,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-680719616"/>
+        <c:crossAx val="811201584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-680719616"/>
+        <c:axId val="811201584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -521,7 +649,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-680721248"/>
+        <c:crossAx val="811215728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -770,11 +898,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-680728320"/>
-        <c:axId val="-680727776"/>
+        <c:axId val="683824304"/>
+        <c:axId val="994535136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-680728320"/>
+        <c:axId val="683824304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,12 +959,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-680727776"/>
+        <c:crossAx val="994535136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-680727776"/>
+        <c:axId val="994535136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,7 +1021,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-680728320"/>
+        <c:crossAx val="683824304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -916,6 +1044,589 @@
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Force [N] as function of Voltage [V]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Calibration_9V_Battery!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Arduino Volt. [N]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Calibration_9V_Battery!$F$2:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.46</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.44</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.41</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Calibration_9V_Battery!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>428.69700000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>428.69700000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>428.69700000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>320.78700000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>320.78700000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>320.78700000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>462.05100000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>462.05100000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>462.05100000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>441.45000000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>441.45000000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>441.45000000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>296.7525</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>296.7525</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>296.7525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="994538400"/>
+        <c:axId val="994540032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="994538400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Voltage Measured [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="994540032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="994540032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Force [N]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="994538400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1022,6 +1733,12 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2050,6 +2767,485 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2122,6 +3318,243 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Calibration_9V_Battery"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="F1" t="str">
+            <v>Arduino Volt. [N]</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="D2">
+            <v>0</v>
+          </cell>
+          <cell r="F2">
+            <v>0.71</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="D3">
+            <v>0</v>
+          </cell>
+          <cell r="F3">
+            <v>0.69</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="D4">
+            <v>0</v>
+          </cell>
+          <cell r="F4">
+            <v>0.69</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="D5">
+            <v>0</v>
+          </cell>
+          <cell r="F5">
+            <v>0.7</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="D6">
+            <v>0</v>
+          </cell>
+          <cell r="F6">
+            <v>0.7</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="D7">
+            <v>428.69700000000006</v>
+          </cell>
+          <cell r="F7">
+            <v>2.34</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="D8">
+            <v>428.69700000000006</v>
+          </cell>
+          <cell r="F8">
+            <v>2.33</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="D9">
+            <v>428.69700000000006</v>
+          </cell>
+          <cell r="F9">
+            <v>2.34</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="D10">
+            <v>320.78700000000003</v>
+          </cell>
+          <cell r="F10">
+            <v>1.94</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="D11">
+            <v>320.78700000000003</v>
+          </cell>
+          <cell r="F11">
+            <v>1.95</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="D12">
+            <v>320.78700000000003</v>
+          </cell>
+          <cell r="F12">
+            <v>1.93</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="D13">
+            <v>462.05100000000004</v>
+          </cell>
+          <cell r="F13">
+            <v>2.4500000000000002</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="D14">
+            <v>462.05100000000004</v>
+          </cell>
+          <cell r="F14">
+            <v>2.46</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="D15">
+            <v>462.05100000000004</v>
+          </cell>
+          <cell r="F15">
+            <v>2.44</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="D16">
+            <v>441.45000000000005</v>
+          </cell>
+          <cell r="F16">
+            <v>2.41</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="D17">
+            <v>441.45000000000005</v>
+          </cell>
+          <cell r="F17">
+            <v>2.39</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="D18">
+            <v>441.45000000000005</v>
+          </cell>
+          <cell r="F18">
+            <v>2.38</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="D19">
+            <v>296.7525</v>
+          </cell>
+          <cell r="F19">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="D20">
+            <v>296.7525</v>
+          </cell>
+          <cell r="F20">
+            <v>1.81</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="D21">
+            <v>296.7525</v>
+          </cell>
+          <cell r="F21">
+            <v>1.79</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:F21"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Weigth [Kg]" dataDxfId="4"/>
+    <tableColumn id="2" name="Force [N]" dataDxfId="3">
+      <calculatedColumnFormula>9.81*A2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Weigth/2 [Kg]" dataDxfId="2">
+      <calculatedColumnFormula>A2/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Force/2 [N]" dataDxfId="1">
+      <calculatedColumnFormula>B2/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Arduino Int []"/>
+    <tableColumn id="6" name="Arduino Volt. [N]" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3977,8 +5410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5066,4 +6499,535 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="11">
+        <f>SLOPE(Table1[Force/2 '[N']],Table1[Arduino Volt. '[N']])</f>
+        <v>261.74271716876274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <f t="shared" ref="B2:B21" si="0">9.81*A2</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <f t="shared" ref="C2:D21" si="1">A2/2</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>146</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="13">
+        <f>INTERCEPT(Table1[Force/2 '[N']],Table1[Arduino Volt. '[N']])</f>
+        <v>-181.94804986838255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>142</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="15">
+        <f>RSQ(Table1[Force/2 '[N']],Table1[Arduino Volt. '[N']])</f>
+        <v>0.99937298346790659</v>
+      </c>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>143</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>144</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>144</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>87.4</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>857.39400000000012</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="1"/>
+        <v>43.7</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="1"/>
+        <v>428.69700000000006</v>
+      </c>
+      <c r="E7">
+        <v>479</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>87.4</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>857.39400000000012</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="1"/>
+        <v>43.7</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="1"/>
+        <v>428.69700000000006</v>
+      </c>
+      <c r="E8">
+        <v>477</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>87.4</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>857.39400000000012</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="1"/>
+        <v>43.7</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>428.69700000000006</v>
+      </c>
+      <c r="E9">
+        <v>479</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>641.57400000000007</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="1"/>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
+        <v>320.78700000000003</v>
+      </c>
+      <c r="E10">
+        <v>396</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>641.57400000000007</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="1"/>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>320.78700000000003</v>
+      </c>
+      <c r="E11">
+        <v>401</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>641.57400000000007</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="1"/>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>320.78700000000003</v>
+      </c>
+      <c r="E12">
+        <v>395</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>94.2</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>924.10200000000009</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="1"/>
+        <v>47.1</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>462.05100000000004</v>
+      </c>
+      <c r="E13">
+        <v>510</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>94.2</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>924.10200000000009</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="1"/>
+        <v>47.1</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="1"/>
+        <v>462.05100000000004</v>
+      </c>
+      <c r="E14">
+        <v>504</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>94.2</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>924.10200000000009</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="1"/>
+        <v>47.1</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="1"/>
+        <v>462.05100000000004</v>
+      </c>
+      <c r="E15">
+        <v>500</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>90</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>882.90000000000009</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="1"/>
+        <v>441.45000000000005</v>
+      </c>
+      <c r="E16">
+        <v>494</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>90</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>882.90000000000009</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="1"/>
+        <v>441.45000000000005</v>
+      </c>
+      <c r="E17">
+        <v>490</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>90</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>882.90000000000009</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="1"/>
+        <v>441.45000000000005</v>
+      </c>
+      <c r="E18">
+        <v>488</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>60.5</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>593.505</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="1"/>
+        <v>30.25</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="1"/>
+        <v>296.7525</v>
+      </c>
+      <c r="E19">
+        <v>370</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>60.5</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>593.505</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="1"/>
+        <v>30.25</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="1"/>
+        <v>296.7525</v>
+      </c>
+      <c r="E20">
+        <v>371</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>60.5</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>593.505</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="1"/>
+        <v>30.25</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="1"/>
+        <v>296.7525</v>
+      </c>
+      <c r="E21">
+        <v>368</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1.79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>